<commit_message>
added zeiten to srcs -F
</commit_message>
<xml_diff>
--- a/AdditionalContent/Planungspraesentation/Wocheneinteilung.xlsx
+++ b/AdditionalContent/Planungspraesentation/Wocheneinteilung.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+  <si>
+    <t>25 Juni - 15 Juli</t>
+  </si>
   <si>
     <t>Lukas</t>
   </si>
@@ -31,6 +34,9 @@
     <t>Spielwelt kann prozedural Generiert werden.</t>
   </si>
   <si>
+    <t>16 Juli - 5 Aug</t>
+  </si>
+  <si>
     <t>Planeten können abgeschossen werden.</t>
   </si>
   <si>
@@ -46,6 +52,9 @@
     <t>Szenenbeleuchtung für die Welt wird installiert.</t>
   </si>
   <si>
+    <t>6 Aug - 26 Aug</t>
+  </si>
+  <si>
     <t>Raumschiff wird modelliert.</t>
   </si>
   <si>
@@ -64,10 +73,19 @@
     <t>Kamera wird (spielgerecht) in der Szene angeordnet.</t>
   </si>
   <si>
+    <t>27 Aug - 16 Sep</t>
+  </si>
+  <si>
     <t>Alle</t>
   </si>
   <si>
     <t>Planeten werden modelliert.</t>
+  </si>
+  <si>
+    <t>16 - 23 September</t>
+  </si>
+  <si>
+    <t>Polishing und Vorbereitung der Abgabe</t>
   </si>
 </sst>
 </file>
@@ -89,7 +107,7 @@
       <color rgb="FF000000"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +136,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
       </patternFill>
     </fill>
   </fills>
@@ -127,16 +151,16 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -147,6 +171,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -174,118 +201,139 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="24.14"/>
     <col customWidth="1" min="2" max="2" width="71.29"/>
+    <col customWidth="1" min="3" max="3" width="70.14"/>
   </cols>
   <sheetData>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="5">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
       <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
+      <c r="B12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>14</v>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>16</v>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>